<commit_message>
altering back the cs and onera
</commit_message>
<xml_diff>
--- a/InputExport.xlsx
+++ b/InputExport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hn17219120-my.sharepoint.com/personal/admin_hn17219120_onmicrosoft_com/Documents/oneraShare/DATABASE_TRIAL/python files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4738" documentId="8_{15C99C78-D71E-471B-887F-F3CB5D345EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5446EDC-9080-40C0-AB89-328256AF5549}"/>
+  <xr:revisionPtr revIDLastSave="4755" documentId="8_{15C99C78-D71E-471B-887F-F3CB5D345EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{552FD8DE-10C4-4168-B77D-A131318CDA80}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EF2D689A-8164-4E18-BACF-DAEC0F75D250}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EF2D689A-8164-4E18-BACF-DAEC0F75D250}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>型號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,15 +105,9 @@
     <t>T116.617.11.057.01</t>
   </si>
   <si>
-    <t>T120.417.11.041.01</t>
-  </si>
-  <si>
     <t>T120.417.11.091.01</t>
   </si>
   <si>
-    <t>T126.010.11.013.00</t>
-  </si>
-  <si>
     <t>T126.010.22.013.01</t>
   </si>
   <si>
@@ -135,17 +129,7 @@
     <t>T41.1.183.33</t>
   </si>
   <si>
-    <t>T41.1.123.57</t>
-  </si>
-  <si>
-    <t>T109.410.11.072.00</t>
-  </si>
-  <si>
-    <t>C106 (SAHS) 0.60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C106 (SAHS) 0.56</t>
+    <t>C107 (SAHS) 0.60</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -236,7 +220,6 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="136"/>
     </font>
     <font>
       <b/>
@@ -388,7 +371,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -410,13 +393,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -752,10 +732,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0290E59D-3F69-470D-93D3-15BFC3940755}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -789,124 +769,124 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
-        <v>20</v>
+      <c r="B2">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="9">
+        <v>21</v>
+      </c>
+      <c r="D2" s="7">
         <v>3180</v>
       </c>
       <c r="E2" s="3">
         <f>D2/B2</f>
-        <v>159</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8">
-        <v>20</v>
+      <c r="B3">
+        <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="9">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7">
         <v>3180</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E20" si="0">D3/B3</f>
-        <v>159</v>
+        <f t="shared" ref="E3:E16" si="0">D3/B3</f>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8">
-        <v>20</v>
+      <c r="B4">
+        <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="9">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7">
         <v>2880</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
-        <v>15</v>
+      <c r="B5">
+        <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="9">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7">
         <v>2880</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8">
-        <v>15</v>
+      <c r="B6">
+        <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="9">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7">
         <v>1680</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8">
-        <v>10</v>
+      <c r="B7">
+        <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7">
         <v>4020</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>402</v>
+        <v>804</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="9">
+        <v>21</v>
+      </c>
+      <c r="D8" s="7">
         <v>1920</v>
       </c>
       <c r="E8" s="3">
@@ -915,52 +895,52 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8">
-        <v>10</v>
+      <c r="B9">
+        <v>5</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="9">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7">
         <v>2790</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>279</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2790</v>
+        <v>21</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2250</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>558</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="9">
+        <v>21</v>
+      </c>
+      <c r="D11" s="7">
         <v>2040</v>
       </c>
       <c r="E11" s="3">
@@ -969,168 +949,93 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="9">
-        <v>2250</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3540</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>708</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="8">
-        <v>15</v>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="9">
-        <v>2040</v>
+        <v>21</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3330</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>136</v>
+        <f>D13/B13</f>
+        <v>3330</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="8">
-        <v>15</v>
+      <c r="B14">
+        <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="9">
-        <v>3540</v>
+        <v>21</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3330</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
-        <v>236</v>
+        <f>D14/B14</f>
+        <v>1110</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8">
-        <v>9</v>
+      <c r="B15">
+        <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="9">
-        <v>3330</v>
+        <v>21</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1770</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
-        <v>370</v>
+        <f>D15/B15</f>
+        <v>590</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="8">
-        <v>7</v>
+      <c r="B16">
+        <v>5</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="9">
-        <v>3330</v>
+        <v>21</v>
+      </c>
+      <c r="D16" s="7">
+        <v>2910</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>475.71428571428572</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="8">
-        <v>12</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1770</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="0"/>
-        <v>147.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="8">
-        <v>10</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="9">
-        <v>2910</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="0"/>
-        <v>291</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="9">
-        <v>2464.0000000000005</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="0"/>
-        <v>1232.0000000000002</v>
-      </c>
-      <c r="F19">
-        <v>32636578</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="8">
-        <v>15</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="9">
-        <v>1260.0000000000002</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="0"/>
-        <v>84.000000000000014</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug in vba that cant close existing wb
</commit_message>
<xml_diff>
--- a/InputExport.xlsx
+++ b/InputExport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hn17219120-my.sharepoint.com/personal/admin_hn17219120_onmicrosoft_com/Documents/oneraShare/DATABASE_TRIAL/python files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4755" documentId="8_{15C99C78-D71E-471B-887F-F3CB5D345EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{552FD8DE-10C4-4168-B77D-A131318CDA80}"/>
+  <xr:revisionPtr revIDLastSave="4760" documentId="8_{15C99C78-D71E-471B-887F-F3CB5D345EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29245354-44BB-4538-8238-30B422E45B39}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EF2D689A-8164-4E18-BACF-DAEC0F75D250}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>型號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,52 +84,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T006.407.16.053.00</t>
+    <t>T109.410.11.072.00</t>
   </si>
   <si>
-    <t>T006.407.11.033.00</t>
-  </si>
-  <si>
-    <t>T006.407.11.053.00</t>
-  </si>
-  <si>
-    <t>T006.407.16.033.00</t>
-  </si>
-  <si>
-    <t>T094.210.11.111.00</t>
-  </si>
-  <si>
-    <t>T099.407.11.048.00</t>
-  </si>
-  <si>
-    <t>T116.617.11.057.01</t>
-  </si>
-  <si>
-    <t>T120.417.11.091.01</t>
-  </si>
-  <si>
-    <t>T126.010.22.013.01</t>
-  </si>
-  <si>
-    <t>T126.010.36.013.00</t>
-  </si>
-  <si>
-    <t>T126.207.11.013.00</t>
-  </si>
-  <si>
-    <t>T137.407.11.041.00</t>
-  </si>
-  <si>
-    <t>T137.407.11.051.00</t>
-  </si>
-  <si>
-    <t>T137.410.11.041.00</t>
-  </si>
-  <si>
-    <t>T41.1.183.33</t>
-  </si>
-  <si>
-    <t>C107 (SAHS) 0.60</t>
+    <t>23/11/2023 POP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -140,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;HK$&quot;* #,##0.00_);_(&quot;HK$&quot;* \(#,##0.00\);_(&quot;HK$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +178,7 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <charset val="136"/>
     </font>
     <font>
       <b/>
@@ -248,7 +207,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF00B0F0"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -371,7 +337,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -393,10 +359,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -732,10 +701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0290E59D-3F69-470D-93D3-15BFC3940755}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -770,272 +739,20 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" s="7">
-        <v>3180</v>
-      </c>
-      <c r="E2" s="3">
-        <f>D2/B2</f>
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="7">
-        <v>3180</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E16" si="0">D3/B3</f>
-        <v>318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2880</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="0"/>
-        <v>288</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2880</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>576</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1680</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4020</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="0"/>
-        <v>804</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1920</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>384</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="7">
-        <v>2790</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="0"/>
-        <v>558</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="7">
-        <v>2250</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="7">
-        <v>2040</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="0"/>
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3540</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>708</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="7">
-        <v>3330</v>
-      </c>
-      <c r="E13" s="3">
-        <f>D13/B13</f>
-        <v>3330</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="7">
-        <v>3330</v>
-      </c>
-      <c r="E14" s="3">
-        <f>D14/B14</f>
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="7">
-        <v>1770</v>
-      </c>
-      <c r="E15" s="3">
-        <f>D15/B15</f>
-        <v>590</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="7">
-        <v>2910</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="0"/>
-        <v>582</v>
+        <v>1119</v>
+      </c>
+      <c r="E2" s="3" t="e">
+        <f>#REF!/B2</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding some more info to 自作單
</commit_message>
<xml_diff>
--- a/InputExport.xlsx
+++ b/InputExport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hn17219120-my.sharepoint.com/personal/admin_hn17219120_onmicrosoft_com/Documents/oneraShare/DATABASE_TRIAL/python files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4941" documentId="8_{15C99C78-D71E-471B-887F-F3CB5D345EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E109EFAD-2922-466E-B211-21C50E0D9427}"/>
+  <xr:revisionPtr revIDLastSave="5363" documentId="8_{15C99C78-D71E-471B-887F-F3CB5D345EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCB086F6-A3AE-4B43-A249-6193BE1109C9}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="720" windowWidth="20025" windowHeight="15480" xr2:uid="{EF2D689A-8164-4E18-BACF-DAEC0F75D250}"/>
+    <workbookView xWindow="1170" yWindow="720" windowWidth="20025" windowHeight="15480" xr2:uid="{EF2D689A-8164-4E18-BACF-DAEC0F75D250}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>型號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,11 +84,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T126.010.36.013.00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C108 (SAHS) 0.60</t>
+    <t>H52414130</t>
+  </si>
+  <si>
+    <t>T41.1.123.57</t>
+  </si>
+  <si>
+    <t>H70545540</t>
+  </si>
+  <si>
+    <t>T063.209.16.038.00</t>
+  </si>
+  <si>
+    <t>C032.607.11.051.00</t>
+  </si>
+  <si>
+    <t>11/12/2023 POP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,7 +190,6 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="136"/>
     </font>
     <font>
       <b/>
@@ -699,10 +709,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0290E59D-3F69-470D-93D3-15BFC3940755}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -740,17 +750,73 @@
         <v>6</v>
       </c>
       <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>3889</v>
+      </c>
+      <c r="E2" s="3" t="e">
+        <f>#REF!/B2</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>4989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>2040</v>
-      </c>
-      <c r="E2" s="3">
-        <f>D2/B2</f>
-        <v>204</v>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>4749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>